<commit_message>
Bold last row in each monthly report
</commit_message>
<xml_diff>
--- a/notebooks/example_output.xlsx
+++ b/notebooks/example_output.xlsx
@@ -518,11 +518,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3646,17 +3647,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>1235</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>2340</v>
       </c>
     </row>
@@ -4302,17 +4303,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>3293</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>282</v>
       </c>
     </row>
@@ -4958,17 +4959,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>537</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>3038</v>
       </c>
     </row>
@@ -5836,17 +5837,17 @@
         <v>-718</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>2198</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1377</v>
       </c>
     </row>
@@ -6492,17 +6493,17 @@
         <v>-86</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>3236</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>339</v>
       </c>
     </row>
@@ -7148,17 +7149,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>2302</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1273</v>
       </c>
     </row>
@@ -7804,17 +7805,17 @@
         <v>-632</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>2520</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1055</v>
       </c>
     </row>
@@ -8460,17 +8461,17 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>1892</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1683</v>
       </c>
     </row>
@@ -9116,17 +9117,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>1791</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>1784</v>
       </c>
     </row>
@@ -9772,17 +9773,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" t="s">
-        <v>144</v>
-      </c>
-      <c r="C38">
+    <row r="38" spans="1:5" s="2" customFormat="1">
+      <c r="A38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" s="2">
         <v>1316</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="2">
         <v>3575</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="2">
         <v>2259</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add autofit logic to write_report_to_excel()
</commit_message>
<xml_diff>
--- a/notebooks/example_output.xlsx
+++ b/notebooks/example_output.xlsx
@@ -823,6 +823,16 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
@@ -3017,6 +3027,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -3673,6 +3690,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -4329,6 +4353,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -4985,6 +5016,11 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -5207,6 +5243,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -5863,6 +5906,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -6519,6 +6569,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -7175,6 +7232,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -7831,6 +7895,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -8487,6 +8558,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
@@ -9143,6 +9221,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">

</xml_diff>